<commit_message>
update Portfolio Overview file
</commit_message>
<xml_diff>
--- a/stock_smr.xlsx
+++ b/stock_smr.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
   <si>
     <t>share</t>
   </si>
@@ -23,27 +23,9 @@
     <t>category</t>
   </si>
   <si>
-    <t>SLV</t>
-  </si>
-  <si>
     <t>VDE</t>
   </si>
   <si>
-    <t>ALLY</t>
-  </si>
-  <si>
-    <t>SGG</t>
-  </si>
-  <si>
-    <t>VIXY</t>
-  </si>
-  <si>
-    <t>DAL</t>
-  </si>
-  <si>
-    <t>KWEB</t>
-  </si>
-  <si>
     <t>STOCK</t>
   </si>
   <si>
@@ -65,15 +47,6 @@
     <t>OIL</t>
   </si>
   <si>
-    <t>FINANCE</t>
-  </si>
-  <si>
-    <t>SUGGAR</t>
-  </si>
-  <si>
-    <t>VIX-INDEX</t>
-  </si>
-  <si>
     <t>SPACE</t>
   </si>
   <si>
@@ -92,9 +65,6 @@
     <t>ENB.TO</t>
   </si>
   <si>
-    <t>BMO.TO</t>
-  </si>
-  <si>
     <t>CASH</t>
   </si>
   <si>
@@ -122,7 +92,7 @@
     <t>products</t>
   </si>
   <si>
-    <t>AIL-LINE</t>
+    <t>HZU.TO</t>
   </si>
 </sst>
 </file>
@@ -464,92 +434,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="C2">
-        <v>29.4</v>
+        <v>12.37</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3">
-        <v>110</v>
+        <v>109.17</v>
       </c>
       <c r="C3">
-        <v>9.27</v>
+        <v>36.64</v>
       </c>
       <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B4">
-        <v>206</v>
+        <v>90</v>
       </c>
       <c r="C4">
-        <v>18.78</v>
+        <v>23.41</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -557,259 +530,119 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>135</v>
+        <v>57</v>
       </c>
       <c r="C5">
-        <v>15.98</v>
+        <v>51.82</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B6">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="C6">
-        <v>51.82</v>
+        <v>32.54</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B7">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="C7">
-        <v>73.25</v>
+        <v>36.119999999999997</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B8">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>36.119999999999997</v>
+        <v>26798</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B9">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>19.190000000000001</v>
+        <v>17208</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B10">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C10">
-        <v>15.57</v>
+        <v>16.940000000000001</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11">
-        <v>20</v>
-      </c>
-      <c r="C11">
-        <v>38.909999999999997</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12">
-        <v>30</v>
-      </c>
-      <c r="C12">
-        <v>25.62</v>
-      </c>
-      <c r="D12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13">
-        <v>15</v>
-      </c>
-      <c r="C13">
-        <v>71.67</v>
-      </c>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14">
-        <v>50</v>
-      </c>
-      <c r="C14">
-        <v>27.64</v>
-      </c>
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15">
-        <v>70</v>
-      </c>
-      <c r="C15">
-        <v>16.940000000000001</v>
-      </c>
-      <c r="D15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>19861.009999999998</v>
-      </c>
-      <c r="D16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>6501.56</v>
-      </c>
-      <c r="D17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -832,25 +665,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="G1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>